<commit_message>
Added Details of 2 students in the excel file
</commit_message>
<xml_diff>
--- a/myexcel.xlsx
+++ b/myexcel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -31,6 +31,12 @@
   </si>
   <si>
     <t>Karan</t>
+  </si>
+  <si>
+    <t>Roshni</t>
+  </si>
+  <si>
+    <t>Jyoti</t>
   </si>
 </sst>
 </file>
@@ -369,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -408,6 +414,28 @@
       </c>
       <c r="C3">
         <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>